<commit_message>
Update SESSION 04 - React + Nodejs
</commit_message>
<xml_diff>
--- a/Homeworks/Mongodb/Database Design & Questions.xlsx
+++ b/Homeworks/Mongodb/Database Design & Questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngothanhtung/GitHub/Aptech/nodejs-tutorials/Homeworks/Mongodb/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonywoo/GitHub/Aptech/nodejs-tutorials/Homeworks/Mongodb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53767A34-62A4-F84A-837C-114E7E8B31D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5178AF5-C49A-7F4A-B7CC-A885D71795A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="126040" yWindow="500" windowWidth="32360" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHẦN I Tables" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="118">
   <si>
     <t>No.</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>Check Discount BETWEEN 0 AND 75</t>
+  </si>
+  <si>
+    <t>categories</t>
   </si>
 </sst>
 </file>
@@ -1141,8 +1144,8 @@
   </sheetPr>
   <dimension ref="A1:Z884"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView topLeftCell="A27" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26499,8 +26502,8 @@
   </sheetPr>
   <dimension ref="A1:Z1007"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -27390,7 +27393,7 @@
         <v>107</v>
       </c>
       <c r="D26" s="80" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E26" s="80"/>
       <c r="F26" s="80"/>

</xml_diff>